<commit_message>
Se crea ejemplo de ejecución exitosa para API
</commit_message>
<xml_diff>
--- a/BaseAPI/src/test/resources/datadriven/BaseDataDriven.xlsx
+++ b/BaseAPI/src/test/resources/datadriven/BaseDataDriven.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/jsanchbe_emeal_nttdata_com/Documents/Escritorio/Ecopetrol/Devops/BaseAutomation/BaseAPI/src/test/resources/datadriven/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{DF29B8EF-655B-479F-BC5A-EF8C74A3648E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D336C95-B57E-4711-A5A8-FE61678B2D0A}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{DF29B8EF-655B-479F-BC5A-EF8C74A3648E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72994A4C-AD0F-43B5-9B0A-4E28205203E8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="869" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="869" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Escenario1" sheetId="4" r:id="rId1"/>
     <sheet name="Escenario2" sheetId="7" r:id="rId2"/>
     <sheet name="EjemploExitoso" sheetId="8" r:id="rId3"/>
-    <sheet name="EjemploFallido" sheetId="9" r:id="rId4"/>
-    <sheet name="datos" sheetId="3" state="hidden" r:id="rId5"/>
+    <sheet name="KPI" sheetId="10" r:id="rId4"/>
+    <sheet name="EjemploFallido" sheetId="9" r:id="rId5"/>
+    <sheet name="datos" sheetId="3" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Escenario1!$A$1:$A$46</definedName>
@@ -117,6 +118,52 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={9C9AC5B2-35D8-495D-95D2-99E107DE1ACF}</author>
+    <author>tc={789A657B-E8F1-4B96-9637-29418A89C064}</author>
+    <author>tc={59E0A895-C3D4-4422-ABEB-C11478F13D36}</author>
+    <author>tc={0E1E207B-B27D-45F8-BBD0-886ACCCA1516}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{9C9AC5B2-35D8-495D-95D2-99E107DE1ACF}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Conservar valor consecutivo como texto</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="1" shapeId="0" xr:uid="{789A657B-E8F1-4B96-9637-29418A89C064}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Por favor no modificar. Valor base, KPI</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="2" shapeId="0" xr:uid="{59E0A895-C3D4-4422-ABEB-C11478F13D36}">
+      <text>
+        <t xml:space="preserve">[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Por favor no modificar. Valor base, QA
+</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="3" shapeId="0" xr:uid="{0E1E207B-B27D-45F8-BBD0-886ACCCA1516}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    ID de KPI para consultar. No aplica para creacion</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>Jhon Andres Sanchez Bermudez</author>
   </authors>
   <commentList>
@@ -139,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="158">
   <si>
     <t>Caso</t>
   </si>
@@ -601,13 +648,25 @@
   </si>
   <si>
     <t>Ambiente</t>
+  </si>
+  <si>
+    <t>Perfil</t>
+  </si>
+  <si>
+    <t>idTransaccion</t>
+  </si>
+  <si>
+    <t>KPI</t>
+  </si>
+  <si>
+    <t>dd85cb30-a9e5-4583-be32-8ab956cb0285</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -650,8 +709,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -670,6 +742,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -685,7 +769,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -695,6 +779,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -715,7 +804,9 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Jose Oliver Herrera Rodriguez" id="{4A30EC9B-6A4C-4BE9-A5AA-0896AA90D3AF}" userId="S::jherrodr@emeal.nttdata.com::b4dea0dc-3084-4de5-bb2c-7caa95f8a342" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -979,6 +1070,24 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2023-05-29T17:54:58.55" personId="{4A30EC9B-6A4C-4BE9-A5AA-0896AA90D3AF}" id="{9C9AC5B2-35D8-495D-95D2-99E107DE1ACF}" done="1">
+    <text>Conservar valor consecutivo como texto</text>
+  </threadedComment>
+  <threadedComment ref="B1" dT="2023-05-29T17:56:21.13" personId="{4A30EC9B-6A4C-4BE9-A5AA-0896AA90D3AF}" id="{789A657B-E8F1-4B96-9637-29418A89C064}" done="1">
+    <text>Por favor no modificar. Valor base, KPI</text>
+  </threadedComment>
+  <threadedComment ref="C1" dT="2023-07-17T20:56:45.18" personId="{4A30EC9B-6A4C-4BE9-A5AA-0896AA90D3AF}" id="{59E0A895-C3D4-4422-ABEB-C11478F13D36}" done="1">
+    <text xml:space="preserve">Por favor no modificar. Valor base, QA
+</text>
+  </threadedComment>
+  <threadedComment ref="D1" dT="2023-06-20T21:26:02.13" personId="{4A30EC9B-6A4C-4BE9-A5AA-0896AA90D3AF}" id="{0E1E207B-B27D-45F8-BBD0-886ACCCA1516}" done="1">
+    <text>ID de KPI para consultar. No aplica para creacion</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517ED666-F427-4B05-AD29-97BE26E8FA33}">
   <dimension ref="A1:E46"/>
@@ -1284,7 +1393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63920A4-CC06-4515-A1D9-B0E632AA7FCC}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1346,6 +1455,58 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C88AF6-4262-4529-AD58-66FB4DC703DE}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{F87BBF88-6CD9-4B9E-B096-151F3D92731E}">
+      <formula1>"QA"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{9C5409F8-9B68-44F2-ADFD-CDACFB1F1CA8}">
+      <formula1>"KPI"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26029BE8-C534-4516-A9A7-E0B16AD7461D}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1395,7 +1556,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F0C869F-D833-4E45-A6CC-21A1D829B8F8}">
   <dimension ref="A1:V31"/>
   <sheetViews>
@@ -1997,26 +2158,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c5abdf2c-8a16-4886-be54-ed4e62a70697">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="6dcff6fb-c744-4b82-8f0b-4ce71711ce53" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009263D68DC986354AA92EC9047B5038EB" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="f0fc7e6aef46ec809f6e445356902ed4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c5abdf2c-8a16-4886-be54-ed4e62a70697" xmlns:ns3="6dcff6fb-c744-4b82-8f0b-4ce71711ce53" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfe9d55b7a83ace495aa0670d0536b79" ns2:_="" ns3:_="">
     <xsd:import namespace="c5abdf2c-8a16-4886-be54-ed4e62a70697"/>
@@ -2219,26 +2360,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABF929D3-10AB-4E3C-8DD6-925C7C3F2BB5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c5abdf2c-8a16-4886-be54-ed4e62a70697"/>
-    <ds:schemaRef ds:uri="6dcff6fb-c744-4b82-8f0b-4ce71711ce53"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C92B58EC-22A6-4E3C-8F79-6DC894C45947}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c5abdf2c-8a16-4886-be54-ed4e62a70697">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="6dcff6fb-c744-4b82-8f0b-4ce71711ce53" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BAEAE49-7210-4672-A178-C5B35DBE9EC7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2257,6 +2399,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C92B58EC-22A6-4E3C-8F79-6DC894C45947}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABF929D3-10AB-4E3C-8DD6-925C7C3F2BB5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c5abdf2c-8a16-4886-be54-ed4e62a70697"/>
+    <ds:schemaRef ds:uri="6dcff6fb-c744-4b82-8f0b-4ce71711ce53"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{3048dc87-43f0-4100-9acb-ae1971c79395}" enabled="0" method="" siteId="{3048dc87-43f0-4100-9acb-ae1971c79395}" removed="1"/>

</xml_diff>

<commit_message>
Commit con Framework base
</commit_message>
<xml_diff>
--- a/BaseAPI/src/test/resources/datadriven/BaseDataDriven.xlsx
+++ b/BaseAPI/src/test/resources/datadriven/BaseDataDriven.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/jsanchbe_emeal_nttdata_com/Documents/Escritorio/Ecopetrol/Devops/BaseAutomation/BaseAPI/src/test/resources/datadriven/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{DF29B8EF-655B-479F-BC5A-EF8C74A3648E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72994A4C-AD0F-43B5-9B0A-4E28205203E8}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{DF29B8EF-655B-479F-BC5A-EF8C74A3648E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5370EF40-F822-444A-A05B-7D4AD167C7D1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="869" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="869" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Escenario1" sheetId="4" r:id="rId1"/>
@@ -186,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="164">
   <si>
     <t>Caso</t>
   </si>
@@ -660,13 +660,31 @@
   </si>
   <si>
     <t>dd85cb30-a9e5-4583-be32-8ab956cb0285</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -715,12 +733,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1393,8 +1405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63920A4-CC06-4515-A1D9-B0E632AA7FCC}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1456,10 +1468,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C88AF6-4262-4529-AD58-66FB4DC703DE}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1492,7 +1504,53 @@
         <v>157</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{F87BBF88-6CD9-4B9E-B096-151F3D92731E}">
       <formula1>"QA"</formula1>
@@ -2158,6 +2216,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009263D68DC986354AA92EC9047B5038EB" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="f0fc7e6aef46ec809f6e445356902ed4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c5abdf2c-8a16-4886-be54-ed4e62a70697" xmlns:ns3="6dcff6fb-c744-4b82-8f0b-4ce71711ce53" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfe9d55b7a83ace495aa0670d0536b79" ns2:_="" ns3:_="">
     <xsd:import namespace="c5abdf2c-8a16-4886-be54-ed4e62a70697"/>
@@ -2360,15 +2427,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2381,6 +2439,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C92B58EC-22A6-4E3C-8F79-6DC894C45947}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BAEAE49-7210-4672-A178-C5B35DBE9EC7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2395,14 +2461,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C92B58EC-22A6-4E3C-8F79-6DC894C45947}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>